<commit_message>
added progress bar and file names
</commit_message>
<xml_diff>
--- a/Caneng_test2.xlsx
+++ b/Caneng_test2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,12 +500,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>112994-030-45-01_R0.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ROLLED BASE ANGLE</t>
+          <t>Rolled Base Angle</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,39 +515,39 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>83 lbs</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>112994-030-45-01_R0.pdf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PL  3/16 x 104 1/4 x 243 7/8</t>
+          <t>Angle bar</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>112994-030-45-02</t>
+          <t>112994-030-45-01</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1314</t>
+          <t>0 lbs</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -564,246 +564,246 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>112994-030-45-02_R0.pdf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ROLLED BASE ANGLE</t>
+          <t>Rolled Plate</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>112994-030-45-03</t>
+          <t>112994-030-45-02</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>657 lbs</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>100555-025-22-01_R0.pdf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HSS RECT 2 1/2 X 1 1/2 X 1/8 X 104 1/4 LG</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>112994-030-45-04</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>180401-076-05-00.pdf</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SHEET 16 GAUGE x 24 1/8 x 45</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>112994-030-45-12</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>700232-001-45-03.pdf</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SHEET 16 GAUGE x 24 1/8 x 30</t>
+          <t>Bracket</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>112994-030-46-04</t>
+          <t>700232-001-45-03</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>218</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>Aluminum</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>700232-001-45-03.pdf</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HHMB 1/2 - 13 UNC x 1 3/4 c/w 2 NUTS &amp; FW'S</t>
+          <t>Support Beam</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>112994-030-46-05</t>
+          <t>700232-001-45-03</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>Steel</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>314</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>file_name</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>HHMB 5/8 - 11 UNC x 2 1/4 c/w 2 NUTS &amp; FW'S</t>
+          <t>description</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>112994-030-45-13</t>
+          <t>part_number</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>weight</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>material</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>quantity</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HHMB 1/2 - 13 UNC x 2 c/w 2 NUTS &amp; FW'S</t>
+          <t>ROLLED BASE ANGLE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>112994-030-45-14</t>
+          <t>112994-030-45-03</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>FLAT WASHER REGULAR 1/2 GRADE 5 MIN</t>
+          <t>PL 3/16 x 104 1/16 x 243 7/8</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Flat Washer Type B Regular_AI</t>
+          <t>112994-030-46-01</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1612</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -813,34 +813,34 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>112994-030-45-00.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RD BAR 3/8 X 11-1/8 LG.</t>
+          <t>ROLLED BASE ANGLE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>112994-030-39-11</t>
+          <t>112994-030-46-03</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -852,22 +852,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>112994-030-45-01.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>L3x2x0.25</t>
+          <t>SHEET 16 GAUGE x 24 1/8 x 30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>112994-030-45-01</t>
+          <t>112994-030-46-04</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>435</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -877,179 +877,179 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>112994-030-45-01.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FB 1 3/4 X 1/4</t>
+          <t>HSS RECT 2 1/2 X 1 1/2 X 1/8 X 104 1/16 LG</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>112994-030-45-01</t>
+          <t>112994-030-46-02</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>468</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>112994-030-45-02.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>PL 3/16 X 30 9/16 X 114 3/16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>112994-030-46-07</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>247</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>112994-030-45-03.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HHMB 1/2- 13 UNC x 1 3/4 c/w 2 NUTS &amp; FW's</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>112994-030-46-05</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>288</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>112994-030-45-04.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HHMB 1/2- 13 UNC x 2 c/w 2 NUTS &amp; FW's</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>112994-030-45-14</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>112994-030-45-05.pdf</t>
+          <t>112994-030-46-00.pdf</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HHMB 5/8- 11 UNC x 2 1/4 c/w 2 NUTS &amp; FW's</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>112994-030-46-06</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>54</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>112994-030-45-06.pdf</t>
+          <t>112994-030-45-03.pdf</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>L3x2x0.25</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1059,29 +1059,29 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>83</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-03.pdf</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>FB 1 3/4 X 1 3/4</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1091,17 +1091,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1113,763 +1113,123 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> description</t>
+          <t>description</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> part_number</t>
+          <t>part_number</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> weight</t>
+          <t>weight</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> material</t>
+          <t>material</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> quantity</t>
+          <t>quantity</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>112994-030-45-02_R0.pdf</t>
+          <t>112994-030-46-01_R0.pdf</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PL 3/16 x 104 1/4 x 243 7/8</t>
+          <t>PL 3/16 x 104 1/16 x 243 7/8</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N/A</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 657</t>
+          <t>806</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> C.S.</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>112994-030-45-03_R0.pdf</t>
+          <t>112994-031-46-01_R0.pdf</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> L3x2x0.25</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N/A</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 83</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> C.S.</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>112994-030-45-03_R0.pdf</t>
+          <t>112994-046-R2.pdf</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FB 1 3/4 X 1 3/4</t>
+          <t>Detail View A (1 : 12) Rolling Tolerance 9 16 Thr</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N/A</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0</t>
+          <t>806</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> C.S.</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>file_name</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>part_number</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>material</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>quantity</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>ROLLED BASE ANGLE</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>112994-030-45-03</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>166</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>ASTM A36</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>PL 3/16 x 104 1/16 x 243 7/8</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>112994-030-46-01</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>1612</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>ROLLED BASE ANGLE</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>112994-030-46-03</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>166</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>ASTM A36</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>SHEET 16 GAUGE x 24 1/8 x 30</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>112994-030-46-04</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>435</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>HSS RECT 2 1/2 X 1 1/2 X 1/8 X 104 1/16 LG</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>112994-030-46-02</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>468</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>ASTM A36</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>PL 3/16 X 30 9/16 X 114 3/16</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>112994-030-46-07</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>247</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>HHMB 1/2- 13 UNC x 1 3/4 c/w 2 NUTS &amp; FW's</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>112994-030-46-05</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>288</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>HHMB 1/2- 13 UNC x 2 c/w 2 NUTS &amp; FW's</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>112994-030-45-14</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>112994-030-46-00_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>HHMB 5/8- 11 UNC x 2 1/4 c/w 2 NUTS &amp; FW's</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>112994-030-46-06</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>112994-030-46-01_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>PL 3/16 x 104 1/16 x 243 7/8</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>806</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
           <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>112994-030-46-07_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>PL 1/4 x 12 x 36</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>112994-030-46-08_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>HHMS 1/4-20 x 3/4 c/w Lock Washer</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>112994-030-46-08</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>112994-030-46-09_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Sheet Metal 20 GA x 18 x 24</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>112994-030-46-09</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>112994-030-46-10_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Tube 1 x 1/8 x 10 ft</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>112994-030-46-10</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>ASTM A500</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>112994-030-46-11_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>DOOR FRAME ASSY</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>112994-030-46-11</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>112994-030-46-12_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>HANDLE WITH GRIP</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>112994-030-46-12</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Plastic</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>file_name</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> description</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> part_number</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> weight</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> material</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> quantity</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>112994-030-46-03_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> L3x2x0.25</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N/A</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 83 lbs</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> C.S.</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>112994-030-46-03_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> FB 1 3/4 X 1/4</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> N/A</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> C.S.</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added progress bar component--- still working on it
</commit_message>
<xml_diff>
--- a/Caneng_test2.xlsx
+++ b/Caneng_test2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,12 +500,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>112994-030-45-01_R0.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rolled Base Angle</t>
+          <t>ROLLED BASE ANGLE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,39 +515,39 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>83 lbs</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>112994-030-45-01_R0.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Angle bar</t>
+          <t>PL  3/16 x 104 1/4 x 243 7/8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>112994-030-45-01</t>
+          <t>112994-030-45-02</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0 lbs</t>
+          <t>1314</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -564,246 +564,246 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>112994-030-45-02_R0.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rolled Plate</t>
+          <t>ROLLED BASE ANGLE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>112994-030-45-02</t>
+          <t>112994-030-45-03</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>657 lbs</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>100555-025-22-01_R0.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HSS RECT 2 1/2 X 1 1/2 X 1/8 X 104 1/4 LG</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>112994-030-45-04</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>468</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>180401-076-05-00.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>SHEET 16 GAUGE x 24 1/8 x 45</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>112994-030-45-12</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>327</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>700232-001-45-03.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bracket</t>
+          <t>SHEET 16 GAUGE x 24 1/8 x 30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>700232-001-45-03</t>
+          <t>112994-030-46-04</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>218</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Aluminum</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>700232-001-45-03.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Support Beam</t>
+          <t>HHMB 1/2- 13 UNC x 1 3/4 c/w 2 NUTS &amp; FW's</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>700232-001-45-03</t>
+          <t>112994-030-46-05</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Steel</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>314</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>file_name</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>HHMB 5/8- 11 UNC x 2 1/4 c/w 2 NUTS &amp; FW's</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>part_number</t>
+          <t>112994-030-45-13</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>weight</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>material</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>quantity</t>
+          <t>24</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ROLLED BASE ANGLE</t>
+          <t>HHMB 1/2- 13 UNC x 2 c/w 2 NUTS &amp; FW's</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>112994-030-45-03</t>
+          <t>112994-030-45-14</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>PL 3/16 x 104 1/16 x 243 7/8</t>
+          <t>CLEVIS PIN WITH HAIRPIN COTTER 1/2 DIAMETER X 1-1/4 LONG 1 USABLE LENGTH</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>112994-030-46-01</t>
+          <t>112994-030-45-15</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1612</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -813,61 +813,61 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ROLLED BASE ANGLE</t>
+          <t>FLAT WASHER REGULAR 1/2 GRADE 5 MIN Flat Washer Type B Regular AI</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>112994-030-46-03</t>
+          <t>112994-030-45-11</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>80</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SHEET 16 GAUGE x 24 1/8 x 30</t>
+          <t>RD BAR 3/8 X 11-1/8 LG</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>112994-030-46-04</t>
+          <t>112994-030-39-11</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>435</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -877,61 +877,61 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-01_R0.pdf</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>HSS RECT 2 1/2 X 1 1/2 X 1/8 X 104 1/16 LG</t>
+          <t>L3x2x0.25</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>112994-030-46-02</t>
+          <t>112994-030-45-01</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>83</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>C.S.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-01_R0.pdf</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PL 3/16 X 30 9/16 X 114 3/16</t>
+          <t>FB 1 3/4 X 1/4</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>112994-030-46-07</t>
+          <t>112994-030-45-02</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -941,61 +941,61 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>file_name</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>HHMB 1/2- 13 UNC x 1 3/4 c/w 2 NUTS &amp; FW's</t>
+          <t>description</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>112994-030-46-05</t>
+          <t>part_number</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>weight</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>material</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>288</t>
+          <t>quantity</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-02_R0.pdf</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>HHMB 1/2- 13 UNC x 2 c/w 2 NUTS &amp; FW's</t>
+          <t>PL  3/16 x 104 1/4 x 243 7/8</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>112994-030-45-14</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>657</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1005,29 +1005,29 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>112994-030-46-00.pdf</t>
+          <t>112994-030-45-03_R0.pdf</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>HHMB 5/8- 11 UNC x 2 1/4 c/w 2 NUTS &amp; FW's</t>
+          <t>L3x2x0.25</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>112994-030-46-06</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>83</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1037,19 +1037,19 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>112994-030-45-03.pdf</t>
+          <t>112994-030-45-03_R0.pdf</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>L3x2x0.25</t>
+          <t>FB 1 3/4 X 1 3/4</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1069,167 +1069,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>112994-030-45-03.pdf</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>FB 1 3/4 X 1 3/4</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
           <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>file_name</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>part_number</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>material</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>quantity</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>112994-030-46-01_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>PL 3/16 x 104 1/16 x 243 7/8</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>806</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>112994-031-46-01_R0.pdf</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>112994-046-R2.pdf</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Detail View A (1 : 12) Rolling Tolerance 9 16 Thr</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>806</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>C.S.</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed styling and workflow
</commit_message>
<xml_diff>
--- a/Caneng_test2.xlsx
+++ b/Caneng_test2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,56 +500,512 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>112994-030-45-01_R0.pdf</t>
+          <t>112994-030-45-00_R0.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>L3x2x0.25</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>ROLLED BASE ANGLE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>112994-030-45-01</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>C.S.</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PL 3/16 x 104 1/4 x 243 7/8</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>112994-030-45-02</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1314</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ROLLED BASE ANGLE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>112994-030-45-03</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>HSS RECT 2 1/2 X 1 1/2 X 1/8 X 104 1/4 LG</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>112994-030-45-04</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>468</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SHEET 16 GAUGE x 24 1/8 x 45</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>112994-030-45-12</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>327</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SHEET 16 GAUGE x 24 1/8 x 30</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>112994-030-46-04</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>218</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>HHMB 1/2- 13 UNC x 1 3/4 c/w 2 NUTS &amp; FW's</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>112994-030-46-05</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>314</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>HHMB 5/8- 11 UNC x 2 1/4 c/w 2 NUTS &amp; FW's</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>112994-030-45-13</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HHMB 1/2- 13 UNC x 2 c/w 2 NUTS &amp; FW's</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>112994-030-45-14</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CLEVIS PIN WITH HAIRPIN COTTER 1/2 DIAMETER X 1-1/4 LONG 1 USABLE LENGTH</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>112994-030-45-15</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FLAT WASHER REGULAR 1/2 GRADE 5 MIN.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>112994-030-45-00_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>RD BAR 3/8 X 11-1/8 LG</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>112994-030-39-11</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>112994-030-45-01_R0.pdf</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>L3x2x0.25</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>C.S.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>112994-030-45-01_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>FB 1 3/4 X 1/4</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>C.S.</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>part_number</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>material</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>112994-030-45-02_R0.pdf</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PLATE STEEL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>112994-030-45-02</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>657</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>PL 3/16 x 104 1/4 x 243 7/8</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>